<commit_message>
Add fx to generate DSS scripts
</commit_message>
<xml_diff>
--- a/OpenPy_fx_tools_dss/IMEX_to_DSS/xlsx_DSS_xlsx/Examples/13NodeIEEE/DSSHelp_Default.xlsx
+++ b/OpenPy_fx_tools_dss/IMEX_to_DSS/xlsx_DSS_xlsx/Examples/13NodeIEEE/DSSHelp_Default.xlsx
@@ -5,21 +5,22 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\GitHub\py-fx-tools-dss\py_fx_tools_dss\IMEX_to_DSS\xlsx_DSS_xlsx\Examples\13NodeIEEE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\GitHub\OpenPy-fx-tools-DSS\openpy_fx_tools_dss\IMEX_to_DSS\xlsx_DSS_xlsx\Examples\13NodeIEEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2FDFF6-C4E5-407B-8643-F9A420452D66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC98D19-EEF1-4C50-9BA1-7E5483FBB357}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2100" yWindow="2565" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Principal" sheetId="5" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="7" r:id="rId2"/>
-    <sheet name="Hoja1" sheetId="6" r:id="rId3"/>
-    <sheet name="DSSHelp" sheetId="1" r:id="rId4"/>
+    <sheet name="Hoja3" sheetId="8" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="7" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="6" r:id="rId4"/>
+    <sheet name="DSSHelp" sheetId="1" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">DSSHelp!$B$1:$Q$132</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">DSSHelp!$B$1:$Q$132</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Principal!$A$1:$O$1694</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15115" uniqueCount="3735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15142" uniqueCount="3735">
   <si>
     <t>Object = EXECUTIVE</t>
   </si>
@@ -11733,7 +11734,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -11773,9 +11774,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -12136,10 +12134,10 @@
   <dimension ref="A1:F1694"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D580" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D381" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E580" sqref="E580"/>
+      <selection pane="bottomRight" activeCell="F580" sqref="F580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16720,14 +16718,14 @@
         <v>847</v>
       </c>
     </row>
-    <row r="381" spans="1:6" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A381" s="5" t="s">
         <v>2945</v>
       </c>
       <c r="D381" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E381"/>
+      <c r="E381" s="1"/>
       <c r="F381" s="9" t="s">
         <v>849</v>
       </c>
@@ -17200,7 +17198,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="421" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A421" s="5" t="s">
         <v>3062</v>
       </c>
@@ -17213,7 +17211,9 @@
       <c r="D421" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E421"/>
+      <c r="E421" s="1">
+        <v>3</v>
+      </c>
       <c r="F421" s="9" t="s">
         <v>927</v>
       </c>
@@ -18136,7 +18136,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="473" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A473" s="5" t="s">
         <v>3062</v>
       </c>
@@ -18149,7 +18149,7 @@
       <c r="D473" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E473"/>
+      <c r="E473" s="1"/>
       <c r="F473" s="9" t="s">
         <v>1031</v>
       </c>
@@ -18550,7 +18550,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="496" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A496" s="5" t="s">
         <v>3062</v>
       </c>
@@ -18563,7 +18563,9 @@
       <c r="D496" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E496"/>
+      <c r="E496" s="1">
+        <v>3</v>
+      </c>
       <c r="F496" s="9" t="s">
         <v>1069</v>
       </c>
@@ -18964,7 +18966,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="519" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A519" s="5" t="s">
         <v>3062</v>
       </c>
@@ -18977,7 +18979,7 @@
       <c r="D519" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E519"/>
+      <c r="E519" s="1"/>
       <c r="F519" s="9" t="s">
         <v>1104</v>
       </c>
@@ -19612,7 +19614,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="555" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A555" s="5" t="s">
         <v>3062</v>
       </c>
@@ -19625,7 +19627,7 @@
       <c r="D555" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E555"/>
+      <c r="E555" s="1"/>
       <c r="F555" s="9" t="s">
         <v>1031</v>
       </c>
@@ -20075,14 +20077,14 @@
       <c r="D580" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E580" s="1">
+      <c r="E580" s="5">
         <v>3</v>
       </c>
       <c r="F580" s="9" t="s">
         <v>1205</v>
       </c>
     </row>
-    <row r="581" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A581" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20095,7 +20097,7 @@
       <c r="D581" s="5" t="s">
         <v>3069</v>
       </c>
-      <c r="E581" s="1">
+      <c r="E581" s="5">
         <v>2</v>
       </c>
       <c r="F581" s="9" t="s">
@@ -20115,7 +20117,7 @@
       <c r="D582" s="5" t="s">
         <v>3070</v>
       </c>
-      <c r="E582"/>
+      <c r="E582" s="1"/>
       <c r="F582" s="9" t="s">
         <v>1207</v>
       </c>
@@ -20133,12 +20135,12 @@
       <c r="D583" s="5" t="s">
         <v>3071</v>
       </c>
-      <c r="E583"/>
+      <c r="E583" s="1"/>
       <c r="F583" s="9" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="584" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A584" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20151,7 +20153,7 @@
       <c r="D584" s="5" t="s">
         <v>3072</v>
       </c>
-      <c r="E584" s="1" t="s">
+      <c r="E584" s="5" t="s">
         <v>3725</v>
       </c>
       <c r="F584" s="9" t="s">
@@ -20171,12 +20173,12 @@
       <c r="D585" s="5" t="s">
         <v>3073</v>
       </c>
-      <c r="E585"/>
+      <c r="E585" s="1"/>
       <c r="F585" s="9" t="s">
         <v>1209</v>
       </c>
     </row>
-    <row r="586" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A586" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20189,7 +20191,6 @@
       <c r="D586" s="5" t="s">
         <v>3074</v>
       </c>
-      <c r="E586" s="1"/>
       <c r="F586" s="9" t="s">
         <v>1210</v>
       </c>
@@ -20207,7 +20208,7 @@
       <c r="D587" s="5" t="s">
         <v>3075</v>
       </c>
-      <c r="E587"/>
+      <c r="E587" s="1"/>
       <c r="F587" s="9" t="s">
         <v>941</v>
       </c>
@@ -20225,12 +20226,12 @@
       <c r="D588" s="5" t="s">
         <v>3076</v>
       </c>
-      <c r="E588"/>
+      <c r="E588" s="1"/>
       <c r="F588" s="9" t="s">
         <v>1211</v>
       </c>
     </row>
-    <row r="589" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A589" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20243,7 +20244,7 @@
       <c r="D589" s="5" t="s">
         <v>3177</v>
       </c>
-      <c r="E589" s="1">
+      <c r="E589" s="5">
         <v>-1</v>
       </c>
       <c r="F589" s="9" t="s">
@@ -20263,7 +20264,7 @@
       <c r="D590" s="5" t="s">
         <v>3178</v>
       </c>
-      <c r="E590"/>
+      <c r="E590" s="1"/>
       <c r="F590" s="9" t="s">
         <v>1215</v>
       </c>
@@ -20281,7 +20282,7 @@
       <c r="D591" s="5" t="s">
         <v>632</v>
       </c>
-      <c r="E591"/>
+      <c r="E591" s="1"/>
       <c r="F591" s="9" t="s">
         <v>1216</v>
       </c>
@@ -20299,7 +20300,7 @@
       <c r="D592" s="5" t="s">
         <v>3079</v>
       </c>
-      <c r="E592"/>
+      <c r="E592" s="1"/>
       <c r="F592" s="9" t="s">
         <v>1217</v>
       </c>
@@ -20317,7 +20318,7 @@
       <c r="D593" s="5" t="s">
         <v>3080</v>
       </c>
-      <c r="E593"/>
+      <c r="E593" s="1"/>
       <c r="F593" s="9" t="s">
         <v>1218</v>
       </c>
@@ -20335,7 +20336,7 @@
       <c r="D594" s="5" t="s">
         <v>3081</v>
       </c>
-      <c r="E594"/>
+      <c r="E594" s="1"/>
       <c r="F594" s="9" t="s">
         <v>955</v>
       </c>
@@ -20353,7 +20354,7 @@
       <c r="D595" s="5" t="s">
         <v>681</v>
       </c>
-      <c r="E595"/>
+      <c r="E595" s="1"/>
       <c r="F595" s="9" t="s">
         <v>957</v>
       </c>
@@ -20371,7 +20372,7 @@
       <c r="D596" s="5" t="s">
         <v>3179</v>
       </c>
-      <c r="E596"/>
+      <c r="E596" s="1"/>
       <c r="F596" s="9" t="s">
         <v>1220</v>
       </c>
@@ -20389,7 +20390,7 @@
       <c r="D597" s="5" t="s">
         <v>3083</v>
       </c>
-      <c r="E597"/>
+      <c r="E597" s="1"/>
       <c r="F597" s="9" t="s">
         <v>1221</v>
       </c>
@@ -20407,7 +20408,7 @@
       <c r="D598" s="5" t="s">
         <v>3180</v>
       </c>
-      <c r="E598"/>
+      <c r="E598" s="1"/>
       <c r="F598" s="9" t="s">
         <v>1223</v>
       </c>
@@ -20425,7 +20426,7 @@
       <c r="D599" s="5" t="s">
         <v>3181</v>
       </c>
-      <c r="E599"/>
+      <c r="E599" s="1"/>
       <c r="F599" s="9" t="s">
         <v>965</v>
       </c>
@@ -20443,7 +20444,9 @@
       <c r="D600" s="5" t="s">
         <v>3086</v>
       </c>
-      <c r="E600"/>
+      <c r="E600" s="1">
+        <v>2</v>
+      </c>
       <c r="F600" s="9" t="s">
         <v>1225</v>
       </c>
@@ -20461,7 +20464,9 @@
       <c r="D601" s="5" t="s">
         <v>3087</v>
       </c>
-      <c r="E601"/>
+      <c r="E601" s="1">
+        <v>0.8</v>
+      </c>
       <c r="F601" s="9" t="s">
         <v>969</v>
       </c>
@@ -20479,12 +20484,14 @@
       <c r="D602" s="5" t="s">
         <v>3088</v>
       </c>
-      <c r="E602"/>
+      <c r="E602" s="1">
+        <v>0.8</v>
+      </c>
       <c r="F602" s="9" t="s">
         <v>971</v>
       </c>
     </row>
-    <row r="603" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A603" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20497,14 +20504,14 @@
       <c r="D603" s="5" t="s">
         <v>3089</v>
       </c>
-      <c r="E603" s="1">
+      <c r="E603" s="5">
         <v>65</v>
       </c>
       <c r="F603" s="9" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="604" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A604" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20517,7 +20524,7 @@
       <c r="D604" s="5" t="s">
         <v>3090</v>
       </c>
-      <c r="E604" s="1">
+      <c r="E604" s="5">
         <v>15</v>
       </c>
       <c r="F604" s="9" t="s">
@@ -20537,12 +20544,12 @@
       <c r="D605" s="5" t="s">
         <v>3091</v>
       </c>
-      <c r="E605"/>
+      <c r="E605" s="1"/>
       <c r="F605" s="9" t="s">
         <v>977</v>
       </c>
     </row>
-    <row r="606" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A606" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20555,14 +20562,14 @@
       <c r="D606" s="5" t="s">
         <v>3092</v>
       </c>
-      <c r="E606" s="1">
+      <c r="E606" s="5">
         <v>0</v>
       </c>
       <c r="F606" s="9" t="s">
         <v>979</v>
       </c>
     </row>
-    <row r="607" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A607" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20575,14 +20582,14 @@
       <c r="D607" s="5" t="s">
         <v>3093</v>
       </c>
-      <c r="E607" s="14" t="s">
+      <c r="E607" s="11" t="s">
         <v>3734</v>
       </c>
       <c r="F607" s="9" t="s">
         <v>1226</v>
       </c>
     </row>
-    <row r="608" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A608" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20595,14 +20602,14 @@
       <c r="D608" s="5" t="s">
         <v>3094</v>
       </c>
-      <c r="E608" s="14" t="s">
+      <c r="E608" s="11" t="s">
         <v>3733</v>
       </c>
       <c r="F608" s="9" t="s">
         <v>1227</v>
       </c>
     </row>
-    <row r="609" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A609" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20615,14 +20622,14 @@
       <c r="D609" s="5" t="s">
         <v>3095</v>
       </c>
-      <c r="E609" s="1" t="s">
+      <c r="E609" s="5" t="s">
         <v>3706</v>
       </c>
       <c r="F609" s="9" t="s">
         <v>1228</v>
       </c>
     </row>
-    <row r="610" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A610" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20635,14 +20642,14 @@
       <c r="D610" s="5" t="s">
         <v>3096</v>
       </c>
-      <c r="E610" s="1">
+      <c r="E610" s="5">
         <v>1.1000000000000001</v>
       </c>
       <c r="F610" s="9" t="s">
         <v>987</v>
       </c>
     </row>
-    <row r="611" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A611" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20655,14 +20662,14 @@
       <c r="D611" s="5" t="s">
         <v>3097</v>
       </c>
-      <c r="E611" s="1">
+      <c r="E611" s="5">
         <v>0.9</v>
       </c>
       <c r="F611" s="9" t="s">
         <v>989</v>
       </c>
     </row>
-    <row r="612" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A612" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20675,14 +20682,14 @@
       <c r="D612" s="5" t="s">
         <v>3098</v>
       </c>
-      <c r="E612" s="1">
+      <c r="E612" s="5">
         <v>32</v>
       </c>
       <c r="F612" s="9" t="s">
         <v>991</v>
       </c>
     </row>
-    <row r="613" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A613" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20695,14 +20702,14 @@
       <c r="D613" s="5" t="s">
         <v>3099</v>
       </c>
-      <c r="E613" s="1" t="s">
+      <c r="E613" s="5" t="s">
         <v>3730</v>
       </c>
       <c r="F613" s="9" t="s">
         <v>993</v>
       </c>
     </row>
-    <row r="614" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A614" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20715,14 +20722,14 @@
       <c r="D614" s="5" t="s">
         <v>3100</v>
       </c>
-      <c r="E614" s="1">
+      <c r="E614" s="5">
         <v>0</v>
       </c>
       <c r="F614" s="9" t="s">
         <v>995</v>
       </c>
     </row>
-    <row r="615" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A615" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20735,7 +20742,7 @@
       <c r="D615" s="5" t="s">
         <v>3101</v>
       </c>
-      <c r="E615" s="1">
+      <c r="E615" s="5">
         <v>1</v>
       </c>
       <c r="F615" s="9" t="s">
@@ -20755,7 +20762,7 @@
       <c r="D616" s="5" t="s">
         <v>3102</v>
       </c>
-      <c r="E616"/>
+      <c r="E616" s="1"/>
       <c r="F616" s="9" t="s">
         <v>1230</v>
       </c>
@@ -20773,7 +20780,7 @@
       <c r="D617" s="5" t="s">
         <v>3103</v>
       </c>
-      <c r="E617"/>
+      <c r="E617" s="1"/>
       <c r="F617" s="9" t="s">
         <v>1001</v>
       </c>
@@ -20791,12 +20798,12 @@
       <c r="D618" s="5" t="s">
         <v>3104</v>
       </c>
-      <c r="E618"/>
+      <c r="E618" s="1"/>
       <c r="F618" s="9" t="s">
         <v>1003</v>
       </c>
     </row>
-    <row r="619" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A619" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20809,7 +20816,7 @@
       <c r="D619" s="5" t="s">
         <v>3105</v>
       </c>
-      <c r="E619" s="1" t="s">
+      <c r="E619" s="5" t="s">
         <v>3706</v>
       </c>
       <c r="F619" s="9" t="s">
@@ -20829,7 +20836,7 @@
       <c r="D620" s="5" t="s">
         <v>3182</v>
       </c>
-      <c r="E620"/>
+      <c r="E620" s="1"/>
       <c r="F620" s="9" t="s">
         <v>1232</v>
       </c>
@@ -20847,7 +20854,7 @@
       <c r="D621" s="5" t="s">
         <v>3183</v>
       </c>
-      <c r="E621"/>
+      <c r="E621" s="1"/>
       <c r="F621" s="9" t="s">
         <v>1234</v>
       </c>
@@ -20865,12 +20872,12 @@
       <c r="D622" s="5" t="s">
         <v>3184</v>
       </c>
-      <c r="E622"/>
+      <c r="E622" s="1"/>
       <c r="F622" s="9" t="s">
         <v>1236</v>
       </c>
     </row>
-    <row r="623" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A623" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20883,7 +20890,7 @@
       <c r="D623" s="5" t="s">
         <v>3106</v>
       </c>
-      <c r="E623" s="1" t="s">
+      <c r="E623" s="5" t="s">
         <v>3731</v>
       </c>
       <c r="F623" s="9" t="s">
@@ -20903,7 +20910,7 @@
       <c r="D624" s="5" t="s">
         <v>3107</v>
       </c>
-      <c r="E624"/>
+      <c r="E624" s="1"/>
       <c r="F624" s="9" t="s">
         <v>1239</v>
       </c>
@@ -20921,12 +20928,12 @@
       <c r="D625" s="5" t="s">
         <v>3078</v>
       </c>
-      <c r="E625"/>
+      <c r="E625" s="1"/>
       <c r="F625" s="9" t="s">
         <v>1241</v>
       </c>
     </row>
-    <row r="626" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A626" s="5" t="s">
         <v>3062</v>
       </c>
@@ -20939,7 +20946,7 @@
       <c r="D626" s="5" t="s">
         <v>3185</v>
       </c>
-      <c r="E626" s="1" t="s">
+      <c r="E626" s="5" t="s">
         <v>3732</v>
       </c>
       <c r="F626" s="9" t="s">
@@ -20959,7 +20966,7 @@
       <c r="D627" s="5" t="s">
         <v>3163</v>
       </c>
-      <c r="E627"/>
+      <c r="E627" s="1"/>
       <c r="F627" s="9" t="s">
         <v>1245</v>
       </c>
@@ -20977,7 +20984,7 @@
       <c r="D628" s="5" t="s">
         <v>3164</v>
       </c>
-      <c r="E628"/>
+      <c r="E628" s="1"/>
       <c r="F628" s="9" t="s">
         <v>1247</v>
       </c>
@@ -20995,7 +21002,7 @@
       <c r="D629" s="5" t="s">
         <v>3108</v>
       </c>
-      <c r="E629"/>
+      <c r="E629" s="1"/>
       <c r="F629" s="9" t="s">
         <v>1011</v>
       </c>
@@ -21013,7 +21020,7 @@
       <c r="D630" s="5" t="s">
         <v>3109</v>
       </c>
-      <c r="E630"/>
+      <c r="E630" s="1"/>
       <c r="F630" s="9" t="s">
         <v>1013</v>
       </c>
@@ -21031,7 +21038,7 @@
       <c r="D631" s="5" t="s">
         <v>3110</v>
       </c>
-      <c r="E631"/>
+      <c r="E631" s="1"/>
       <c r="F631" s="9" t="s">
         <v>1015</v>
       </c>
@@ -21049,7 +21056,7 @@
       <c r="D632" s="5" t="s">
         <v>3111</v>
       </c>
-      <c r="E632"/>
+      <c r="E632" s="1"/>
       <c r="F632" s="9" t="s">
         <v>1017</v>
       </c>
@@ -21067,7 +21074,7 @@
       <c r="D633" s="5" t="s">
         <v>3112</v>
       </c>
-      <c r="E633"/>
+      <c r="E633" s="1"/>
       <c r="F633" s="9" t="s">
         <v>1019</v>
       </c>
@@ -21085,7 +21092,7 @@
       <c r="D634" s="5" t="s">
         <v>3113</v>
       </c>
-      <c r="E634"/>
+      <c r="E634" s="1"/>
       <c r="F634" s="9" t="s">
         <v>1021</v>
       </c>
@@ -21103,7 +21110,7 @@
       <c r="D635" s="5" t="s">
         <v>3114</v>
       </c>
-      <c r="E635"/>
+      <c r="E635" s="1"/>
       <c r="F635" s="9" t="s">
         <v>1023</v>
       </c>
@@ -21121,12 +21128,12 @@
       <c r="D636" s="5" t="s">
         <v>3115</v>
       </c>
-      <c r="E636"/>
+      <c r="E636" s="1"/>
       <c r="F636" s="9" t="s">
         <v>1025</v>
       </c>
     </row>
-    <row r="637" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="637" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A637" s="5" t="s">
         <v>3063</v>
       </c>
@@ -21139,7 +21146,7 @@
       <c r="D637" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E637"/>
+      <c r="E637" s="1"/>
       <c r="F637" s="9" t="s">
         <v>1256</v>
       </c>
@@ -21990,7 +21997,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="685" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="685" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A685" s="5" t="s">
         <v>3063</v>
       </c>
@@ -22003,7 +22010,7 @@
       <c r="D685" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E685"/>
+      <c r="E685" s="1"/>
       <c r="F685" s="9" t="s">
         <v>1347</v>
       </c>
@@ -23016,7 +23023,7 @@
         <v>1447</v>
       </c>
     </row>
-    <row r="742" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="742" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A742" s="5" t="s">
         <v>3063</v>
       </c>
@@ -23029,7 +23036,9 @@
       <c r="D742" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E742"/>
+      <c r="E742" s="1">
+        <v>3</v>
+      </c>
       <c r="F742" s="9" t="s">
         <v>1449</v>
       </c>
@@ -23268,7 +23277,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="756" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="756" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A756" s="5" t="s">
         <v>3063</v>
       </c>
@@ -23281,7 +23290,7 @@
       <c r="D756" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E756"/>
+      <c r="E756" s="1"/>
       <c r="F756" s="9" t="s">
         <v>1347</v>
       </c>
@@ -23718,7 +23727,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="781" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="781" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A781" s="5" t="s">
         <v>3063</v>
       </c>
@@ -23731,7 +23740,7 @@
       <c r="D781" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E781"/>
+      <c r="E781" s="1"/>
       <c r="F781" s="9" t="s">
         <v>1491</v>
       </c>
@@ -24528,7 +24537,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="823" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="823" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A823" s="5" t="s">
         <v>3063</v>
       </c>
@@ -24541,7 +24550,7 @@
       <c r="D823" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E823"/>
+      <c r="E823" s="1"/>
       <c r="F823" s="9" t="s">
         <v>1565</v>
       </c>
@@ -25320,7 +25329,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="867" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="867" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A867" s="5" t="s">
         <v>3063</v>
       </c>
@@ -25333,7 +25342,7 @@
       <c r="D867" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E867"/>
+      <c r="E867" s="1"/>
       <c r="F867" s="9" t="s">
         <v>1643</v>
       </c>
@@ -26400,7 +26409,7 @@
         <v>1749</v>
       </c>
     </row>
-    <row r="927" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A927" s="5" t="s">
         <v>3063</v>
       </c>
@@ -26413,7 +26422,9 @@
       <c r="D927" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E927"/>
+      <c r="E927" s="1">
+        <v>1</v>
+      </c>
       <c r="F927" s="9" t="s">
         <v>1750</v>
       </c>
@@ -26688,7 +26699,7 @@
         <v>1776</v>
       </c>
     </row>
-    <row r="943" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="943" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A943" s="5" t="s">
         <v>3063</v>
       </c>
@@ -26701,7 +26712,9 @@
       <c r="D943" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E943"/>
+      <c r="E943" s="1">
+        <v>1</v>
+      </c>
       <c r="F943" s="9" t="s">
         <v>1778</v>
       </c>
@@ -26976,7 +26989,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="959" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="959" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A959" s="5" t="s">
         <v>3063</v>
       </c>
@@ -26989,7 +27002,9 @@
       <c r="D959" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E959"/>
+      <c r="E959" s="1">
+        <v>4</v>
+      </c>
       <c r="F959" s="9" t="s">
         <v>1806</v>
       </c>
@@ -27390,7 +27405,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="982" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="982" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A982" s="5" t="s">
         <v>3063</v>
       </c>
@@ -27403,7 +27418,7 @@
       <c r="D982" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E982"/>
+      <c r="E982" s="1"/>
       <c r="F982" s="9" t="s">
         <v>1844</v>
       </c>
@@ -33600,7 +33615,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="1328" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1328" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1328" s="5" t="s">
         <v>2976</v>
       </c>
@@ -34118,7 +34133,7 @@
         <v>2466</v>
       </c>
     </row>
-    <row r="1357" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1357" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1357" s="5" t="s">
         <v>2976</v>
       </c>
@@ -34131,7 +34146,9 @@
       <c r="D1357" s="5" t="s">
         <v>3564</v>
       </c>
-      <c r="E1357"/>
+      <c r="E1357" s="1">
+        <v>3</v>
+      </c>
       <c r="F1357" s="9" t="s">
         <v>2468</v>
       </c>
@@ -34478,7 +34495,7 @@
         <v>2502</v>
       </c>
     </row>
-    <row r="1377" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1377" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1377" s="5" t="s">
         <v>2976</v>
       </c>
@@ -34491,7 +34508,7 @@
       <c r="D1377" s="5" t="s">
         <v>3564</v>
       </c>
-      <c r="E1377"/>
+      <c r="E1377" s="1"/>
       <c r="F1377" s="9" t="s">
         <v>2503</v>
       </c>
@@ -36248,7 +36265,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="1475" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1475" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1475" s="5" t="s">
         <v>2976</v>
       </c>
@@ -36261,7 +36278,9 @@
       <c r="D1475" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E1475"/>
+      <c r="E1475" s="1">
+        <v>3</v>
+      </c>
       <c r="F1475" s="9" t="s">
         <v>1205</v>
       </c>
@@ -38765,7 +38784,7 @@
         <v>2823</v>
       </c>
     </row>
-    <row r="1615" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1615" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1615" s="5" t="s">
         <v>2996</v>
       </c>
@@ -38778,7 +38797,9 @@
       <c r="D1615" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E1615"/>
+      <c r="E1615" s="1">
+        <v>1</v>
+      </c>
       <c r="F1615" s="9" t="s">
         <v>2824</v>
       </c>
@@ -39089,7 +39110,7 @@
         <v>2846</v>
       </c>
     </row>
-    <row r="1633" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1633" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1633" s="5" t="s">
         <v>2996</v>
       </c>
@@ -39102,7 +39123,9 @@
       <c r="D1633" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E1633"/>
+      <c r="E1633" s="1">
+        <v>3</v>
+      </c>
       <c r="F1633" s="9" t="s">
         <v>2848</v>
       </c>
@@ -39359,7 +39382,7 @@
         <v>2868</v>
       </c>
     </row>
-    <row r="1648" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1648" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1648" s="5" t="s">
         <v>2996</v>
       </c>
@@ -39372,7 +39395,9 @@
       <c r="D1648" s="5" t="s">
         <v>848</v>
       </c>
-      <c r="E1648"/>
+      <c r="E1648" s="1">
+        <v>3</v>
+      </c>
       <c r="F1648" s="9" t="s">
         <v>2869</v>
       </c>
@@ -39647,7 +39672,7 @@
         <v>2889</v>
       </c>
     </row>
-    <row r="1664" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1664" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1664" s="5" t="s">
         <v>2996</v>
       </c>
@@ -40232,56 +40257,11 @@
       <c r="E1694"/>
     </row>
   </sheetData>
-  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:O1694" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
+  <autoFilter ref="A1:O1694" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="3">
       <filters>
-        <filter val="TRANSFORMER"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="5">
-      <filters>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <x14:filter val="{Lead | Lag (default) | ANSI (default) | Euro } Designation in mixed Delta-wye connections the relationship between HV to LV winding. Default is ANSI 30 deg lag, e.g., Dy1 of Yd1 vector group. To get typical European Dy11 connection, specify either &quot;lead&quot; or &quot;Euro&quot;"/>
-            <x14:filter val="={Yes|No}  Designates whether this transformer is to be considered a substation.Default is No."/>
-            <x14:filter val="={Yes|No} Default is NO. Signifies whether or not the X/R is assumed contant for harmonic studies."/>
-            <x14:filter val="Base kVA rating of the winding. Side effect: forces change of max normal and emerg kVA ratings.If 2-winding transformer, forces other winding to same value. When winding 1 is defined, all other windings are defaulted to the same rating and the first two winding resistances are defaulted to the %loadloss value."/>
-            <x14:filter val="Connection of this winding {wye*, Delta, LN, LL}. Default is &quot;wye&quot; with the neutral solidly grounded."/>
-            <x14:filter val="Default = -1. Neutral resistance of wye (star)-connected winding in actual ohms. If entered as a negative value, the neutral is assumed to be open, or floating. To solidly ground the neutral, connect the neutral conductor to Node 0 in the Bus property spec for this winding. For example: Bus=MyBusName.1.2.3.0, which is generally the default connection."/>
-            <x14:filter val="Default=1 ppm.  Parts per million of transformer winding VA rating connected to ground to protect against accidentally floating a winding without a reference. If positive then the effect is adding a very large reactance to ground.  If negative, then a capacitor."/>
-            <x14:filter val="Emergency (contingency)  kVA rating of H winding (winding 1).  Usually 140% - 150% ofmaximum nameplate rating, depending on load shape. Defaults to 150% of kVA rating of Winding 1."/>
-            <x14:filter val="Hot spot temperature rise, deg C.  Default is 15."/>
-            <x14:filter val="Max per unit tap for the active winding.  Default is 1.10"/>
-            <x14:filter val="Min per unit tap for the active winding.  Default is 0.90"/>
-            <x14:filter val="Normal maximum kVA rating of H winding (winding 1).  Usually 100% - 110% ofmaximum nameplate rating, depending on load shape. Defaults to 110% of kVA rating of Winding 1."/>
-            <x14:filter val="Number of phases this transformer. Default is 3."/>
-            <x14:filter val="Number of windings, this transformers. (Also is the number of terminals) Default is 2. This property triggers memory allocation for the Transformer and will cause other properties to revert to default values."/>
-            <x14:filter val="Percent magnetizing current. Default=0.0. Magnetizing branch is in parallel with windings in each phase. Also, see &quot;ppm_antifloat&quot;."/>
-            <x14:filter val="Percent no load losses at rated excitatation voltage. Default is 0. Converts to a resistance in parallel with the magnetizing impedance in each winding."/>
-            <x14:filter val="Substation Name. Optional. Default is null. If specified, printed on plots"/>
-            <x14:filter val="Temperature rise, deg C, for full load.  Default is 65."/>
-            <x14:filter val="Total number of taps between min and max tap.  Default is 32 (16 raise and 16 lower taps about the neutral position). The neutral position is not counted."/>
-            <x14:filter val="Winding dc resistance in OHMS. Useful for GIC analysis. From transformer test report. Defaults to 85% of %R property"/>
-          </mc:Choice>
-          <mc:Fallback>
-            <filter val="={Yes|No}  Designates whether this transformer is to be considered a substation.Default is No."/>
-            <filter val="={Yes|No} Default is NO. Signifies whether or not the X/R is assumed contant for harmonic studies."/>
-            <filter val="Connection of this winding {wye*, Delta, LN, LL}. Default is &quot;wye&quot; with the neutral solidly grounded."/>
-            <filter val="Emergency (contingency)  kVA rating of H winding (winding 1).  Usually 140% - 150% ofmaximum nameplate rating, depending on load shape. Defaults to 150% of kVA rating of Winding 1."/>
-            <filter val="Hot spot temperature rise, deg C.  Default is 15."/>
-            <filter val="Max per unit tap for the active winding.  Default is 1.10"/>
-            <filter val="Min per unit tap for the active winding.  Default is 0.90"/>
-            <filter val="Normal maximum kVA rating of H winding (winding 1).  Usually 100% - 110% ofmaximum nameplate rating, depending on load shape. Defaults to 110% of kVA rating of Winding 1."/>
-            <filter val="Number of phases this transformer. Default is 3."/>
-            <filter val="Number of windings, this transformers. (Also is the number of terminals) Default is 2. This property triggers memory allocation for the Transformer and will cause other properties to revert to default values."/>
-            <filter val="Percent magnetizing current. Default=0.0. Magnetizing branch is in parallel with windings in each phase. Also, see &quot;ppm_antifloat&quot;."/>
-            <filter val="Percent no load losses at rated excitatation voltage. Default is 0. Converts to a resistance in parallel with the magnetizing impedance in each winding."/>
-            <filter val="Substation Name. Optional. Default is null. If specified, printed on plots"/>
-            <filter val="Temperature rise, deg C, for full load.  Default is 65."/>
-            <filter val="Total number of taps between min and max tap.  Default is 32 (16 raise and 16 lower taps about the neutral position). The neutral position is not counted."/>
-            <filter val="Winding dc resistance in OHMS. Useful for GIC analysis. From transformer test report. Defaults to 85% of %R property"/>
-          </mc:Fallback>
-        </mc:AlternateContent>
+        <filter val="nphases"/>
+        <filter val="phases"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -40291,11 +40271,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1072914-3AB3-4465-8FE6-52A7D0A095E1}">
-  <dimension ref="A1:AB7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBCF528E-AAA4-4C97-9EBC-724EAE634AB1}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1072914-3AB3-4465-8FE6-52A7D0A095E1}">
+  <dimension ref="A1:AB12"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40518,18 +40512,136 @@
         <v>3727</v>
       </c>
     </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>848</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>3069</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>3072</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>3177</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>3089</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>3090</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>3092</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>3093</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>3094</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>3095</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>3096</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>3097</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>3098</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>3099</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>3100</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>3101</v>
+      </c>
+      <c r="Q11" s="5" t="s">
+        <v>3105</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>3106</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>3185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>3</v>
+      </c>
+      <c r="B12" s="5">
+        <v>2</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>3725</v>
+      </c>
+      <c r="D12" s="5">
+        <v>-1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>65</v>
+      </c>
+      <c r="F12" s="5">
+        <v>15</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>3734</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>3733</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>3706</v>
+      </c>
+      <c r="K12" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="M12" s="5">
+        <v>32</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>3730</v>
+      </c>
+      <c r="O12" s="5">
+        <v>0</v>
+      </c>
+      <c r="P12" s="5">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="5" t="s">
+        <v>3706</v>
+      </c>
+      <c r="R12" s="5" t="s">
+        <v>3731</v>
+      </c>
+      <c r="S12" s="5" t="s">
+        <v>3732</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA528E1-F644-4044-97C9-D7CF4F5A7F75}">
   <dimension ref="A1:J1881"/>
   <sheetViews>
     <sheetView topLeftCell="A1881" workbookViewId="0">
-      <selection activeCell="B443" sqref="B443:B1881"/>
+      <selection activeCell="A1881" sqref="A1881"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53912,7 +54024,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q1881"/>
   <sheetViews>

</xml_diff>